<commit_message>
TB-370 Add project proposed unit costs to export test
</commit_message>
<xml_diff>
--- a/jems-ui/e2e/cypress/fixtures/project/exports/partners-budget/TB-370-v4.xlsx
+++ b/jems-ui/e2e/cypress/fixtures/project/exports/partners-budget/TB-370-v4.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\jems\ems\jems-ui\e2e\cypress\fixtures\project\exports\partners-budget\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51E9A605-DFA8-4325-94EF-D4D7A5588A6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B765266-C418-4DD5-AC47-B1AA614D29F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21600" yWindow="1110" windowWidth="27780" windowHeight="15780" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="first_tab" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="117">
   <si>
     <t>D - Project budget</t>
   </si>
@@ -305,9 +305,36 @@
     <t>API generated travel and accommodation cost unit type EN</t>
   </si>
   <si>
+    <t>API generated description of the unit cost EN</t>
+  </si>
+  <si>
+    <t>API generated project proposed travel and accommodation cost comments EN</t>
+  </si>
+  <si>
+    <t>E.2.1_Project Proposed Unit Cost for One Category EN</t>
+  </si>
+  <si>
+    <t>API gen unit type EN</t>
+  </si>
+  <si>
     <t>External expertise and services</t>
   </si>
   <si>
+    <t>API generated external cost description EN</t>
+  </si>
+  <si>
+    <t>API generated external cost comments EN</t>
+  </si>
+  <si>
+    <t>API generated external cost award procedures EN</t>
+  </si>
+  <si>
+    <t>I1.1</t>
+  </si>
+  <si>
+    <t>API generated external cost unit type EN</t>
+  </si>
+  <si>
     <t>Equipment</t>
   </si>
   <si>
@@ -329,6 +356,9 @@
     <t>MCC type EN</t>
   </si>
   <si>
+    <t>E.2.1_Project Proposed Unit Cost for Multi Categories EN</t>
+  </si>
+  <si>
     <t>Staff costs</t>
   </si>
   <si>
@@ -342,18 +372,6 @@
   </si>
   <si>
     <t>Other costs flat rate</t>
-  </si>
-  <si>
-    <t>API generated external cost description EN</t>
-  </si>
-  <si>
-    <t>API generated external cost comments EN</t>
-  </si>
-  <si>
-    <t>API generated external cost award procedures EN</t>
-  </si>
-  <si>
-    <t>API generated external cost unit type EN</t>
   </si>
 </sst>
 </file>
@@ -483,14 +501,14 @@
   </cellStyleXfs>
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
@@ -809,57 +827,55 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AC22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="56.5546875" customWidth="1"/>
-    <col min="2" max="2" width="8.109375" customWidth="1"/>
-    <col min="3" max="3" width="24.33203125" customWidth="1"/>
-    <col min="4" max="4" width="41.77734375" customWidth="1"/>
-    <col min="5" max="5" width="32.77734375" customWidth="1"/>
-    <col min="6" max="6" width="14.5546875" customWidth="1"/>
-    <col min="7" max="7" width="18.6640625" customWidth="1"/>
-    <col min="8" max="8" width="17.88671875" customWidth="1"/>
-    <col min="9" max="9" width="14.44140625" customWidth="1"/>
-    <col min="10" max="10" width="14.5546875" customWidth="1"/>
-    <col min="11" max="11" width="34.5546875" customWidth="1"/>
-    <col min="12" max="12" width="37.44140625" customWidth="1"/>
-    <col min="13" max="13" width="31.21875" customWidth="1"/>
+    <col min="1" max="1" width="46.7109375" customWidth="1"/>
+    <col min="2" max="2" width="8" customWidth="1"/>
+    <col min="3" max="3" width="24.28515625" customWidth="1"/>
+    <col min="4" max="4" width="41.7109375" customWidth="1"/>
+    <col min="5" max="5" width="32.85546875" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" customWidth="1"/>
+    <col min="7" max="7" width="18.7109375" customWidth="1"/>
+    <col min="8" max="8" width="17.85546875" customWidth="1"/>
+    <col min="9" max="9" width="14.42578125" customWidth="1"/>
+    <col min="10" max="10" width="14.5703125" customWidth="1"/>
+    <col min="11" max="11" width="34.5703125" customWidth="1"/>
+    <col min="12" max="12" width="37.42578125" customWidth="1"/>
+    <col min="13" max="13" width="31.28515625" customWidth="1"/>
     <col min="14" max="14" width="33" customWidth="1"/>
-    <col min="15" max="15" width="34.6640625" customWidth="1"/>
-    <col min="16" max="16" width="34.77734375" customWidth="1"/>
-    <col min="17" max="17" width="34.44140625" customWidth="1"/>
-    <col min="18" max="18" width="37.88671875" customWidth="1"/>
+    <col min="15" max="15" width="34.7109375" customWidth="1"/>
+    <col min="16" max="16" width="34.85546875" customWidth="1"/>
+    <col min="17" max="17" width="34.42578125" customWidth="1"/>
+    <col min="18" max="18" width="37.85546875" customWidth="1"/>
     <col min="19" max="19" width="38" customWidth="1"/>
-    <col min="20" max="20" width="23.6640625" customWidth="1"/>
-    <col min="21" max="21" width="20.109375" customWidth="1"/>
-    <col min="22" max="22" width="20.21875" customWidth="1"/>
+    <col min="20" max="20" width="23.7109375" customWidth="1"/>
+    <col min="21" max="21" width="20.140625" customWidth="1"/>
+    <col min="22" max="22" width="20.28515625" customWidth="1"/>
     <col min="23" max="23" width="29" customWidth="1"/>
-    <col min="24" max="24" width="32.44140625" customWidth="1"/>
-    <col min="25" max="25" width="32.5546875" customWidth="1"/>
-    <col min="26" max="26" width="11.33203125" customWidth="1"/>
-    <col min="27" max="27" width="10.33203125" customWidth="1"/>
-    <col min="28" max="28" width="44.21875" customWidth="1"/>
-    <col min="29" max="29" width="19.33203125" customWidth="1"/>
+    <col min="24" max="24" width="32.42578125" customWidth="1"/>
+    <col min="25" max="25" width="32.5703125" customWidth="1"/>
+    <col min="26" max="26" width="11.28515625" customWidth="1"/>
+    <col min="27" max="27" width="10.28515625" customWidth="1"/>
+    <col min="28" max="28" width="44.28515625" customWidth="1"/>
+    <col min="29" max="29" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -921,7 +937,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>22</v>
       </c>
@@ -947,13 +963,13 @@
         <v>29</v>
       </c>
       <c r="I5" s="6">
-        <v>731.14</v>
+        <v>3422.72</v>
       </c>
       <c r="J5" s="6">
         <v>60</v>
       </c>
       <c r="K5" s="6">
-        <v>37.6</v>
+        <v>73.83</v>
       </c>
       <c r="L5" s="6">
         <v>0</v>
@@ -965,7 +981,7 @@
         <v>0</v>
       </c>
       <c r="O5" s="6">
-        <v>487.44</v>
+        <v>2281.8200000000002</v>
       </c>
       <c r="P5" s="6">
         <v>0</v>
@@ -974,16 +990,16 @@
         <v>0</v>
       </c>
       <c r="R5" s="6">
-        <v>487.44</v>
+        <v>2281.8200000000002</v>
       </c>
       <c r="S5" s="6">
-        <v>1218.58</v>
+        <v>5704.54</v>
       </c>
       <c r="T5" s="7">
-        <v>37.6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.3">
+        <v>73.83</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>30</v>
       </c>
@@ -1015,7 +1031,7 @@
         <v>60</v>
       </c>
       <c r="K6" s="6">
-        <v>31.2</v>
+        <v>13.09</v>
       </c>
       <c r="L6" s="6">
         <v>303.35000000000002</v>
@@ -1042,10 +1058,10 @@
         <v>1011.19</v>
       </c>
       <c r="T6" s="7">
-        <v>31.2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.3">
+        <v>13.09</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>38</v>
       </c>
@@ -1077,7 +1093,7 @@
         <v>60</v>
       </c>
       <c r="K7" s="6">
-        <v>31.2</v>
+        <v>13.09</v>
       </c>
       <c r="L7" s="6">
         <v>303.35000000000002</v>
@@ -1104,10 +1120,10 @@
         <v>1011.19</v>
       </c>
       <c r="T7" s="7">
-        <v>31.2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.3">
+        <v>13.09</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>40</v>
       </c>
@@ -1133,7 +1149,7 @@
         <v>41</v>
       </c>
       <c r="I8" s="9">
-        <v>1944.56</v>
+        <v>4636.1400000000003</v>
       </c>
       <c r="J8" s="8" t="s">
         <v>41</v>
@@ -1151,7 +1167,7 @@
         <v>41</v>
       </c>
       <c r="O8" s="9">
-        <v>587.44000000000005</v>
+        <v>2381.8200000000002</v>
       </c>
       <c r="P8" s="9">
         <v>0</v>
@@ -1160,24 +1176,24 @@
         <v>102.26</v>
       </c>
       <c r="R8" s="9">
-        <v>689.7</v>
+        <v>2484.08</v>
       </c>
       <c r="S8" s="9">
-        <v>3240.96</v>
+        <v>7726.92</v>
       </c>
       <c r="T8" s="10">
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>2</v>
       </c>
@@ -1266,7 +1282,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>22</v>
       </c>
@@ -1286,10 +1302,10 @@
         <v>27</v>
       </c>
       <c r="G12" s="6">
-        <v>190.66</v>
+        <v>661.82</v>
       </c>
       <c r="H12" s="6">
-        <v>190.66</v>
+        <v>661.82</v>
       </c>
       <c r="I12" s="6">
         <v>0</v>
@@ -1298,13 +1314,13 @@
         <v>0</v>
       </c>
       <c r="K12" s="6">
-        <v>19.059999999999999</v>
+        <v>66.180000000000007</v>
       </c>
       <c r="L12" s="6">
-        <v>19.059999999999999</v>
+        <v>66.180000000000007</v>
       </c>
       <c r="M12" s="6">
-        <v>100</v>
+        <v>2455.81</v>
       </c>
       <c r="N12" s="6">
         <v>0</v>
@@ -1313,7 +1329,7 @@
         <v>100</v>
       </c>
       <c r="P12" s="6">
-        <v>0</v>
+        <v>2355.81</v>
       </c>
       <c r="Q12" s="6">
         <v>100</v>
@@ -1349,13 +1365,13 @@
         <v>0</v>
       </c>
       <c r="AB12" s="6">
-        <v>55.56</v>
+        <v>1667.43</v>
       </c>
       <c r="AC12" s="7">
-        <v>1218.58</v>
-      </c>
-    </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.3">
+        <v>5704.54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>30</v>
       </c>
@@ -1444,7 +1460,7 @@
         <v>1011.19</v>
       </c>
     </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>38</v>
       </c>
@@ -1533,7 +1549,7 @@
         <v>1011.19</v>
       </c>
     </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>40</v>
       </c>
@@ -1553,10 +1569,10 @@
         <v>41</v>
       </c>
       <c r="G15" s="9">
-        <v>1635.22</v>
+        <v>2106.38</v>
       </c>
       <c r="H15" s="9">
-        <v>190.66</v>
+        <v>661.82</v>
       </c>
       <c r="I15" s="9">
         <v>0</v>
@@ -1565,13 +1581,13 @@
         <v>1444.56</v>
       </c>
       <c r="K15" s="9">
-        <v>19.059999999999999</v>
+        <v>66.180000000000007</v>
       </c>
       <c r="L15" s="9">
-        <v>19.059999999999999</v>
+        <v>66.180000000000007</v>
       </c>
       <c r="M15" s="9">
-        <v>100</v>
+        <v>2455.81</v>
       </c>
       <c r="N15" s="9">
         <v>0</v>
@@ -1580,7 +1596,7 @@
         <v>100</v>
       </c>
       <c r="P15" s="9">
-        <v>0</v>
+        <v>2355.81</v>
       </c>
       <c r="Q15" s="9">
         <v>100</v>
@@ -1616,21 +1632,21 @@
         <v>0</v>
       </c>
       <c r="AB15" s="9">
-        <v>55.56</v>
+        <v>1667.43</v>
       </c>
       <c r="AC15" s="10">
-        <v>3240.96</v>
-      </c>
-    </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.3">
+        <v>7726.92</v>
+      </c>
+    </row>
+    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>2</v>
       </c>
@@ -1686,7 +1702,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>22</v>
       </c>
@@ -1709,7 +1725,7 @@
         <v>0</v>
       </c>
       <c r="H19" s="6">
-        <v>190.12</v>
+        <v>3064.21</v>
       </c>
       <c r="I19" s="6">
         <v>61</v>
@@ -1730,7 +1746,7 @@
         <v>0</v>
       </c>
       <c r="O19" s="6">
-        <v>357.46</v>
+        <v>1969.33</v>
       </c>
       <c r="P19" s="6">
         <v>0</v>
@@ -1739,10 +1755,10 @@
         <v>0</v>
       </c>
       <c r="R19" s="7">
-        <v>1218.58</v>
-      </c>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
+        <v>5704.54</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>30</v>
       </c>
@@ -1798,7 +1814,7 @@
         <v>1011.19</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>38</v>
       </c>
@@ -1854,7 +1870,7 @@
         <v>1011.19</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
         <v>40</v>
       </c>
@@ -1877,7 +1893,7 @@
         <v>0</v>
       </c>
       <c r="H22" s="9">
-        <v>470.12</v>
+        <v>3344.21</v>
       </c>
       <c r="I22" s="9">
         <v>341</v>
@@ -1898,7 +1914,7 @@
         <v>280</v>
       </c>
       <c r="O22" s="9">
-        <v>419.84</v>
+        <v>2031.71</v>
       </c>
       <c r="P22" s="9">
         <v>0</v>
@@ -1907,7 +1923,7 @@
         <v>0</v>
       </c>
       <c r="R22" s="10">
-        <v>3240.96</v>
+        <v>7726.92</v>
       </c>
     </row>
   </sheetData>
@@ -1917,48 +1933,51 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AE14"/>
+  <dimension ref="A1:AE16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="Q7" sqref="Q7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="56.5546875" customWidth="1"/>
-    <col min="2" max="2" width="8.109375" customWidth="1"/>
-    <col min="3" max="3" width="24.33203125" customWidth="1"/>
-    <col min="4" max="4" width="41.77734375" customWidth="1"/>
-    <col min="5" max="5" width="32.77734375" customWidth="1"/>
-    <col min="6" max="6" width="14.5546875" customWidth="1"/>
-    <col min="7" max="7" width="18.6640625" customWidth="1"/>
-    <col min="8" max="8" width="14.21875" customWidth="1"/>
-    <col min="9" max="9" width="44.21875" customWidth="1"/>
-    <col min="10" max="10" width="55.88671875" customWidth="1"/>
-    <col min="11" max="11" width="55.33203125" customWidth="1"/>
-    <col min="12" max="12" width="62.109375" customWidth="1"/>
-    <col min="13" max="13" width="11.21875" customWidth="1"/>
-    <col min="14" max="14" width="20.88671875" customWidth="1"/>
+    <col min="1" max="1" width="46.7109375" customWidth="1"/>
+    <col min="2" max="2" width="8" customWidth="1"/>
+    <col min="3" max="3" width="24.28515625" customWidth="1"/>
+    <col min="4" max="4" width="41.7109375" customWidth="1"/>
+    <col min="5" max="5" width="32.85546875" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" customWidth="1"/>
+    <col min="7" max="7" width="18.7109375" customWidth="1"/>
+    <col min="8" max="8" width="14.28515625" customWidth="1"/>
+    <col min="9" max="9" width="44.28515625" customWidth="1"/>
+    <col min="10" max="10" width="55.85546875" customWidth="1"/>
+    <col min="11" max="11" width="71.140625" customWidth="1"/>
+    <col min="12" max="12" width="47.85546875" customWidth="1"/>
+    <col min="13" max="13" width="11.140625" customWidth="1"/>
+    <col min="14" max="14" width="20.85546875" customWidth="1"/>
     <col min="15" max="15" width="11" customWidth="1"/>
-    <col min="16" max="16" width="17.88671875" customWidth="1"/>
-    <col min="17" max="17" width="53.88671875" customWidth="1"/>
-    <col min="18" max="18" width="11.44140625" customWidth="1"/>
+    <col min="16" max="16" width="52" customWidth="1"/>
+    <col min="17" max="17" width="53.85546875" customWidth="1"/>
+    <col min="18" max="18" width="11.42578125" customWidth="1"/>
     <col min="19" max="19" width="13" customWidth="1"/>
-    <col min="20" max="20" width="11.6640625" customWidth="1"/>
-    <col min="21" max="29" width="8.44140625" customWidth="1"/>
-    <col min="30" max="30" width="7.77734375" customWidth="1"/>
-    <col min="31" max="31" width="8.77734375" customWidth="1"/>
+    <col min="20" max="20" width="11.5703125" customWidth="1"/>
+    <col min="21" max="21" width="8.85546875" customWidth="1"/>
+    <col min="22" max="27" width="8.42578125" customWidth="1"/>
+    <col min="28" max="28" width="8.85546875" customWidth="1"/>
+    <col min="29" max="29" width="8.42578125" customWidth="1"/>
+    <col min="30" max="30" width="7.7109375" customWidth="1"/>
+    <col min="31" max="31" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -2053,7 +2072,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>22</v>
       </c>
@@ -2115,7 +2134,7 @@
         <v>0</v>
       </c>
       <c r="U4" s="6">
-        <v>22.06</v>
+        <v>493.22</v>
       </c>
       <c r="V4" s="6">
         <v>10</v>
@@ -2145,10 +2164,10 @@
         <v>0</v>
       </c>
       <c r="AE4" s="7">
-        <v>190.66</v>
-      </c>
-    </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.3">
+        <v>661.82</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>22</v>
       </c>
@@ -2243,7 +2262,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>22</v>
       </c>
@@ -2269,16 +2288,16 @@
         <v>29</v>
       </c>
       <c r="I6" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="J6" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="J6" s="5" t="s">
-        <v>107</v>
-      </c>
       <c r="K6" s="5" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
       <c r="L6" s="5" t="s">
-        <v>109</v>
+        <v>41</v>
       </c>
       <c r="M6" s="5" t="s">
         <v>41</v>
@@ -2290,22 +2309,22 @@
         <v>0</v>
       </c>
       <c r="P6" s="5" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="Q6" s="5" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="R6" s="6">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="S6" s="6">
-        <v>100</v>
+        <v>123.99</v>
       </c>
       <c r="T6" s="6">
         <v>0</v>
       </c>
       <c r="U6" s="6">
-        <v>50</v>
+        <v>2355.81</v>
       </c>
       <c r="V6" s="6">
         <v>0</v>
@@ -2326,7 +2345,7 @@
         <v>0</v>
       </c>
       <c r="AB6" s="6">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AC6" s="6">
         <v>0</v>
@@ -2335,10 +2354,10 @@
         <v>0</v>
       </c>
       <c r="AE6" s="7">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.3">
+        <v>2355.81</v>
+      </c>
+    </row>
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>22</v>
       </c>
@@ -2364,19 +2383,19 @@
         <v>29</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="K7" s="5" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="L7" s="5" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="M7" s="5" t="s">
-        <v>41</v>
+        <v>102</v>
       </c>
       <c r="N7" s="5" t="s">
         <v>41</v>
@@ -2388,52 +2407,52 @@
         <v>89</v>
       </c>
       <c r="Q7" s="5" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="R7" s="6">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="S7" s="6">
-        <v>150.66</v>
+        <v>100</v>
       </c>
       <c r="T7" s="6">
         <v>0</v>
       </c>
       <c r="U7" s="6">
-        <v>10.3</v>
+        <v>50</v>
       </c>
       <c r="V7" s="6">
+        <v>0</v>
+      </c>
+      <c r="W7" s="6">
+        <v>0</v>
+      </c>
+      <c r="X7" s="6">
+        <v>0</v>
+      </c>
+      <c r="Y7" s="6">
+        <v>0</v>
+      </c>
+      <c r="Z7" s="6">
+        <v>0</v>
+      </c>
+      <c r="AA7" s="6">
+        <v>0</v>
+      </c>
+      <c r="AB7" s="6">
         <v>50</v>
       </c>
-      <c r="W7" s="6">
-        <v>400</v>
-      </c>
-      <c r="X7" s="6">
+      <c r="AC7" s="6">
+        <v>0</v>
+      </c>
+      <c r="AD7" s="6">
+        <v>0</v>
+      </c>
+      <c r="AE7" s="7">
         <v>100</v>
       </c>
-      <c r="Y7" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z7" s="6">
-        <v>0</v>
-      </c>
-      <c r="AA7" s="6">
-        <v>0</v>
-      </c>
-      <c r="AB7" s="6">
-        <v>193</v>
-      </c>
-      <c r="AC7" s="6">
-        <v>0</v>
-      </c>
-      <c r="AD7" s="6">
-        <v>0</v>
-      </c>
-      <c r="AE7" s="7">
-        <v>753.3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>22</v>
       </c>
@@ -2459,52 +2478,52 @@
         <v>29</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>48</v>
+        <v>104</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>41</v>
+        <v>105</v>
       </c>
       <c r="K8" s="5" t="s">
-        <v>41</v>
+        <v>106</v>
       </c>
       <c r="L8" s="5" t="s">
-        <v>41</v>
+        <v>107</v>
       </c>
       <c r="M8" s="5" t="s">
-        <v>41</v>
+        <v>102</v>
       </c>
       <c r="N8" s="5" t="s">
         <v>41</v>
       </c>
       <c r="O8" s="5">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="P8" s="5" t="s">
         <v>89</v>
       </c>
       <c r="Q8" s="5" t="s">
-        <v>41</v>
+        <v>108</v>
       </c>
       <c r="R8" s="6">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="S8" s="6">
-        <v>0</v>
+        <v>150.66</v>
       </c>
       <c r="T8" s="6">
         <v>0</v>
       </c>
       <c r="U8" s="6">
-        <v>2.2000000000000002</v>
+        <v>10.3</v>
       </c>
       <c r="V8" s="6">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="W8" s="6">
-        <v>8</v>
+        <v>400</v>
       </c>
       <c r="X8" s="6">
-        <v>2</v>
+        <v>100</v>
       </c>
       <c r="Y8" s="6">
         <v>0</v>
@@ -2516,7 +2535,7 @@
         <v>0</v>
       </c>
       <c r="AB8" s="6">
-        <v>5.86</v>
+        <v>193</v>
       </c>
       <c r="AC8" s="6">
         <v>0</v>
@@ -2525,10 +2544,10 @@
         <v>0</v>
       </c>
       <c r="AE8" s="7">
-        <v>19.059999999999999</v>
-      </c>
-    </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.3">
+        <v>753.3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>22</v>
       </c>
@@ -2554,129 +2573,129 @@
         <v>29</v>
       </c>
       <c r="I9" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="K9" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="L9" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="M9" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="N9" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="O9" s="5">
+        <v>10</v>
+      </c>
+      <c r="P9" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="Q9" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="R9" s="6">
+        <v>0</v>
+      </c>
+      <c r="S9" s="6">
+        <v>0</v>
+      </c>
+      <c r="T9" s="6">
+        <v>0</v>
+      </c>
+      <c r="U9" s="6">
+        <v>49.32</v>
+      </c>
+      <c r="V9" s="6">
+        <v>1</v>
+      </c>
+      <c r="W9" s="6">
+        <v>8</v>
+      </c>
+      <c r="X9" s="6">
+        <v>2</v>
+      </c>
+      <c r="Y9" s="6">
+        <v>0</v>
+      </c>
+      <c r="Z9" s="6">
+        <v>0</v>
+      </c>
+      <c r="AA9" s="6">
+        <v>0</v>
+      </c>
+      <c r="AB9" s="6">
+        <v>5.86</v>
+      </c>
+      <c r="AC9" s="6">
+        <v>0</v>
+      </c>
+      <c r="AD9" s="6">
+        <v>0</v>
+      </c>
+      <c r="AE9" s="7">
+        <v>66.180000000000007</v>
+      </c>
+    </row>
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="I10" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="J9" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="K9" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="L9" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="M9" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="N9" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="O9" s="5">
-        <v>0</v>
-      </c>
-      <c r="P9" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="Q9" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="R9" s="6">
+      <c r="J10" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="K10" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="L10" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="M10" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="N10" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="O10" s="5">
+        <v>0</v>
+      </c>
+      <c r="P10" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q10" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="R10" s="6">
         <v>1</v>
-      </c>
-      <c r="S9" s="6">
-        <v>55.56</v>
-      </c>
-      <c r="T9" s="6">
-        <v>0</v>
-      </c>
-      <c r="U9" s="6">
-        <v>55.56</v>
-      </c>
-      <c r="V9" s="6">
-        <v>0</v>
-      </c>
-      <c r="W9" s="6">
-        <v>0</v>
-      </c>
-      <c r="X9" s="6">
-        <v>0</v>
-      </c>
-      <c r="Y9" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z9" s="6">
-        <v>0</v>
-      </c>
-      <c r="AA9" s="6">
-        <v>0</v>
-      </c>
-      <c r="AB9" s="6">
-        <v>0</v>
-      </c>
-      <c r="AC9" s="6">
-        <v>0</v>
-      </c>
-      <c r="AD9" s="6">
-        <v>0</v>
-      </c>
-      <c r="AE9" s="7">
-        <v>55.56</v>
-      </c>
-    </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A10" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="H10" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="I10" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="J10" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="K10" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="L10" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="M10" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="N10" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="O10" s="5">
-        <v>0</v>
-      </c>
-      <c r="P10" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="Q10" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="R10" s="6">
-        <v>13</v>
       </c>
       <c r="S10" s="6">
         <v>55.56</v>
@@ -2685,28 +2704,28 @@
         <v>0</v>
       </c>
       <c r="U10" s="6">
-        <v>100</v>
+        <v>55.56</v>
       </c>
       <c r="V10" s="6">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="W10" s="6">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="X10" s="6">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="Y10" s="6">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="Z10" s="6">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="AA10" s="6">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="AB10" s="6">
-        <v>22.28</v>
+        <v>0</v>
       </c>
       <c r="AC10" s="6">
         <v>0</v>
@@ -2715,113 +2734,113 @@
         <v>0</v>
       </c>
       <c r="AE10" s="7">
-        <v>722.28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.3">
+        <v>55.56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="K11" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="L11" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="M11" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="N11" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="O11" s="5">
+        <v>0</v>
+      </c>
+      <c r="P11" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q11" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="R11" s="6">
+        <v>13</v>
+      </c>
+      <c r="S11" s="6">
+        <v>123.99</v>
+      </c>
+      <c r="T11" s="6">
+        <v>0</v>
+      </c>
+      <c r="U11" s="6">
+        <v>0</v>
+      </c>
+      <c r="V11" s="6">
+        <v>0</v>
+      </c>
+      <c r="W11" s="6">
+        <v>0</v>
+      </c>
+      <c r="X11" s="6">
+        <v>0</v>
+      </c>
+      <c r="Y11" s="6">
+        <v>0</v>
+      </c>
+      <c r="Z11" s="6">
+        <v>0</v>
+      </c>
+      <c r="AA11" s="6">
+        <v>0</v>
+      </c>
+      <c r="AB11" s="6">
+        <v>1611.87</v>
+      </c>
+      <c r="AC11" s="6">
+        <v>0</v>
+      </c>
+      <c r="AD11" s="6">
+        <v>0</v>
+      </c>
+      <c r="AE11" s="7">
+        <v>1611.87</v>
+      </c>
+    </row>
+    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B12" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C12" s="5" t="s">
         <v>32</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="H11" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="I11" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="J11" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="K11" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="L11" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="M11" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="N11" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="O11" s="5">
-        <v>40</v>
-      </c>
-      <c r="P11" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="Q11" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="R11" s="6">
-        <v>0</v>
-      </c>
-      <c r="S11" s="6">
-        <v>0</v>
-      </c>
-      <c r="T11" s="6">
-        <v>0</v>
-      </c>
-      <c r="U11" s="6">
-        <v>40</v>
-      </c>
-      <c r="V11" s="6">
-        <v>40</v>
-      </c>
-      <c r="W11" s="6">
-        <v>40</v>
-      </c>
-      <c r="X11" s="6">
-        <v>40</v>
-      </c>
-      <c r="Y11" s="6">
-        <v>40</v>
-      </c>
-      <c r="Z11" s="6">
-        <v>40</v>
-      </c>
-      <c r="AA11" s="6">
-        <v>40</v>
-      </c>
-      <c r="AB11" s="6">
-        <v>8.91</v>
-      </c>
-      <c r="AC11" s="6">
-        <v>0</v>
-      </c>
-      <c r="AD11" s="6">
-        <v>0</v>
-      </c>
-      <c r="AE11" s="7">
-        <v>288.91000000000003</v>
-      </c>
-    </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A12" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>39</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>33</v>
@@ -2839,13 +2858,13 @@
         <v>37</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="K12" s="5" t="s">
-        <v>104</v>
+        <v>114</v>
       </c>
       <c r="L12" s="5" t="s">
         <v>41</v>
@@ -2860,10 +2879,10 @@
         <v>0</v>
       </c>
       <c r="P12" s="5" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="Q12" s="5" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="R12" s="6">
         <v>13</v>
@@ -2908,15 +2927,15 @@
         <v>722.28</v>
       </c>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>33</v>
@@ -2934,7 +2953,7 @@
         <v>37</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="J13" s="5" t="s">
         <v>41</v>
@@ -3003,99 +3022,289 @@
         <v>288.91000000000003</v>
       </c>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A14" s="8" t="s">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="J14" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="K14" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="L14" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="M14" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="N14" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="O14" s="5">
+        <v>0</v>
+      </c>
+      <c r="P14" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q14" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="R14" s="6">
+        <v>13</v>
+      </c>
+      <c r="S14" s="6">
+        <v>55.56</v>
+      </c>
+      <c r="T14" s="6">
+        <v>0</v>
+      </c>
+      <c r="U14" s="6">
+        <v>100</v>
+      </c>
+      <c r="V14" s="6">
+        <v>100</v>
+      </c>
+      <c r="W14" s="6">
+        <v>100</v>
+      </c>
+      <c r="X14" s="6">
+        <v>100</v>
+      </c>
+      <c r="Y14" s="6">
+        <v>100</v>
+      </c>
+      <c r="Z14" s="6">
+        <v>100</v>
+      </c>
+      <c r="AA14" s="6">
+        <v>100</v>
+      </c>
+      <c r="AB14" s="6">
+        <v>22.28</v>
+      </c>
+      <c r="AC14" s="6">
+        <v>0</v>
+      </c>
+      <c r="AD14" s="6">
+        <v>0</v>
+      </c>
+      <c r="AE14" s="7">
+        <v>722.28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="J15" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="K15" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="L15" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="M15" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="N15" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="O15" s="5">
         <v>40</v>
       </c>
-      <c r="B14" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="E14" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="F14" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="G14" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="H14" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="I14" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="J14" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="K14" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="L14" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="M14" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="N14" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="O14" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="P14" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q14" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="R14" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="S14" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="T14" s="9">
-        <v>0</v>
-      </c>
-      <c r="U14" s="9">
-        <v>470.12</v>
-      </c>
-      <c r="V14" s="9">
+      <c r="P15" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="Q15" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="R15" s="6">
+        <v>0</v>
+      </c>
+      <c r="S15" s="6">
+        <v>0</v>
+      </c>
+      <c r="T15" s="6">
+        <v>0</v>
+      </c>
+      <c r="U15" s="6">
+        <v>40</v>
+      </c>
+      <c r="V15" s="6">
+        <v>40</v>
+      </c>
+      <c r="W15" s="6">
+        <v>40</v>
+      </c>
+      <c r="X15" s="6">
+        <v>40</v>
+      </c>
+      <c r="Y15" s="6">
+        <v>40</v>
+      </c>
+      <c r="Z15" s="6">
+        <v>40</v>
+      </c>
+      <c r="AA15" s="6">
+        <v>40</v>
+      </c>
+      <c r="AB15" s="6">
+        <v>8.91</v>
+      </c>
+      <c r="AC15" s="6">
+        <v>0</v>
+      </c>
+      <c r="AD15" s="6">
+        <v>0</v>
+      </c>
+      <c r="AE15" s="7">
+        <v>288.91000000000003</v>
+      </c>
+    </row>
+    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="H16" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="I16" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="J16" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="K16" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="L16" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="M16" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="N16" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="O16" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P16" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q16" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="R16" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="S16" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="T16" s="9">
+        <v>0</v>
+      </c>
+      <c r="U16" s="9">
+        <v>3344.21</v>
+      </c>
+      <c r="V16" s="9">
         <v>341</v>
       </c>
-      <c r="W14" s="9">
+      <c r="W16" s="9">
         <v>768</v>
       </c>
-      <c r="X14" s="9">
+      <c r="X16" s="9">
         <v>402</v>
       </c>
-      <c r="Y14" s="9">
+      <c r="Y16" s="9">
         <v>280</v>
       </c>
-      <c r="Z14" s="9">
+      <c r="Z16" s="9">
         <v>280</v>
       </c>
-      <c r="AA14" s="9">
+      <c r="AA16" s="9">
         <v>280</v>
       </c>
-      <c r="AB14" s="9">
-        <v>419.84</v>
-      </c>
-      <c r="AC14" s="9">
-        <v>0</v>
-      </c>
-      <c r="AD14" s="9">
-        <v>0</v>
-      </c>
-      <c r="AE14" s="10">
-        <v>3240.96</v>
+      <c r="AB16" s="9">
+        <v>2031.71</v>
+      </c>
+      <c r="AC16" s="9">
+        <v>0</v>
+      </c>
+      <c r="AD16" s="9">
+        <v>0</v>
+      </c>
+      <c r="AE16" s="10">
+        <v>7726.92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>